<commit_message>
fixed errors and added final checks
</commit_message>
<xml_diff>
--- a/lineage/data/heiser_data/new_version/AU00601_C4_2_1_V4.xlsx
+++ b/lineage/data/heiser_data/new_version/AU00601_C4_2_1_V4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukakarginov/lineage-growth/lineage/data/heiser_data/new_version/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71AA2B5-EB14-D04D-9B9B-A08FFDAB8322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12147E9-3FF7-0D40-945D-73346B1FD403}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -563,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V451"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A288" zoomScale="139" workbookViewId="0">
-      <selection activeCell="P307" sqref="P307"/>
+    <sheetView tabSelected="1" topLeftCell="A266" zoomScale="139" workbookViewId="0">
+      <selection activeCell="N278" activeCellId="1" sqref="G302 N278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="10" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>